<commit_message>
Working with all styles unoptimized
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -38,7 +38,7 @@
       <sz val="10"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill/>
     </fill>
@@ -63,6 +63,12 @@
         <bgColor rgb="00FFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00CCCCCC"/>
+        <bgColor rgb="00CCCCCC"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -82,7 +88,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -91,6 +97,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -891,7 +900,7 @@
       <c r="AG3" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="AH3" s="3" t="n">
+      <c r="AH3" s="4" t="n">
         <v>10</v>
       </c>
       <c r="AI3" s="3" t="n">
@@ -1252,7 +1261,7 @@
       <c r="H7" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="I7" s="3" t="n">
+      <c r="I7" s="4" t="n">
         <v>6</v>
       </c>
       <c r="J7" s="3" t="n">
@@ -1285,7 +1294,7 @@
       <c r="S7" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="T7" s="3" t="n">
+      <c r="T7" s="4" t="n">
         <v>8</v>
       </c>
       <c r="U7" s="3" t="n">
@@ -1324,7 +1333,7 @@
       <c r="AF7" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="AG7" s="3" t="n">
+      <c r="AG7" s="4" t="n">
         <v>10</v>
       </c>
       <c r="AH7" s="3" t="n">
@@ -1357,7 +1366,7 @@
       <c r="L8" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M8" s="3" t="n">
+      <c r="M8" s="4" t="n">
         <v>1</v>
       </c>
       <c r="N8" s="3" t="n">
@@ -1375,7 +1384,7 @@
       <c r="R8" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="S8" s="3" t="n">
+      <c r="S8" s="4" t="n">
         <v>8</v>
       </c>
       <c r="T8" s="3" t="n">
@@ -1506,7 +1515,7 @@
       <c r="I10" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="J10" s="3" t="n">
+      <c r="J10" s="4" t="n">
         <v>6</v>
       </c>
       <c r="K10" s="3" t="n">
@@ -1518,7 +1527,7 @@
       <c r="M10" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="N10" s="3" t="n">
+      <c r="N10" s="4" t="n">
         <v>1</v>
       </c>
       <c r="O10" s="3" t="n">

</xml_diff>